<commit_message>
change excel2json to many
</commit_message>
<xml_diff>
--- a/monitor_xlsx/20260126.xlsx
+++ b/monitor_xlsx/20260126.xlsx
@@ -43,10 +43,10 @@
       <color rgb="00FFFFFF"/>
     </font>
     <font>
-      <color rgb="00FF0000"/>
+      <color rgb="00008000"/>
     </font>
     <font>
-      <color rgb="00008000"/>
+      <color rgb="00FF0000"/>
     </font>
   </fonts>
   <fills count="4">
@@ -745,7 +745,7 @@
       <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr">
         <is>
-          <t>158.39%</t>
+          <t>160.27%</t>
         </is>
       </c>
       <c r="F11" t="inlineStr"/>
@@ -829,12 +829,12 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>-25.97億</t>
+          <t>-24.72億</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>-519.5億</t>
+          <t>-494.44億</t>
         </is>
       </c>
     </row>
@@ -993,7 +993,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>-25.97億</t>
+          <t>-24.72億</t>
         </is>
       </c>
     </row>
@@ -1005,7 +1005,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>-519.5億</t>
+          <t>-494.44億</t>
         </is>
       </c>
     </row>
@@ -1024,7 +1024,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>158.39%</t>
+          <t>160.27%</t>
         </is>
       </c>
     </row>
@@ -1222,15 +1222,27 @@
       <c r="E4" t="n">
         <v>87992</v>
       </c>
+      <c r="F4" s="6" t="n">
+        <v>2647</v>
+      </c>
       <c r="G4" t="n">
         <v>-142411</v>
       </c>
       <c r="I4" t="n">
         <v>-8257</v>
       </c>
+      <c r="J4" t="n">
+        <v>29327</v>
+      </c>
+      <c r="K4" t="n">
+        <v>7044</v>
+      </c>
       <c r="L4" t="n">
         <v>38703</v>
       </c>
+      <c r="M4" t="n">
+        <v>-3953740</v>
+      </c>
       <c r="N4" t="n">
         <v>0.04</v>
       </c>
@@ -1239,27 +1251,9 @@
           <t>主力積極賣出</t>
         </is>
       </c>
-      <c r="P4" t="n">
-        <v>-14</v>
-      </c>
-      <c r="Q4" s="6" t="n">
-        <v>-5.81</v>
-      </c>
-      <c r="R4" t="n">
-        <v>135922000</v>
-      </c>
-      <c r="S4" t="n">
-        <v>1.17</v>
-      </c>
-      <c r="T4" t="n">
-        <v>70.13</v>
-      </c>
-      <c r="U4" t="n">
-        <v>3.02</v>
-      </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t>partial</t>
+          <t>N/A</t>
         </is>
       </c>
     </row>
@@ -1274,41 +1268,38 @@
           <t>S&amp;P黃金正2</t>
         </is>
       </c>
+      <c r="F5" s="6" t="n">
+        <v>8</v>
+      </c>
       <c r="G5" t="n">
         <v>-224</v>
       </c>
+      <c r="H5" t="n">
+        <v>-40</v>
+      </c>
       <c r="I5" t="n">
         <v>-30</v>
       </c>
+      <c r="J5" t="n">
+        <v>4088</v>
+      </c>
+      <c r="K5" t="n">
+        <v>7833</v>
+      </c>
       <c r="L5" t="n">
         <v>35425</v>
       </c>
+      <c r="M5" t="n">
+        <v>-20977</v>
+      </c>
       <c r="O5" t="inlineStr">
         <is>
           <t>主力積極賣出</t>
         </is>
       </c>
-      <c r="P5" t="n">
-        <v>-7</v>
-      </c>
-      <c r="Q5" s="7" t="n">
-        <v>3.59</v>
-      </c>
-      <c r="R5" t="n">
-        <v>533000</v>
-      </c>
-      <c r="S5" t="n">
-        <v>14.29</v>
-      </c>
-      <c r="T5" t="n">
-        <v>102.69</v>
-      </c>
-      <c r="U5" t="n">
-        <v>0</v>
-      </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>partial</t>
+          <t>N/A</t>
         </is>
       </c>
     </row>
@@ -1326,21 +1317,36 @@
       <c r="C6" t="n">
         <v>1020</v>
       </c>
-      <c r="D6" s="7" t="n">
+      <c r="D6" s="6" t="n">
         <v>-0.97</v>
       </c>
       <c r="E6" t="n">
         <v>4393</v>
       </c>
+      <c r="F6" s="6" t="n">
+        <v>748</v>
+      </c>
       <c r="G6" t="n">
         <v>667</v>
       </c>
+      <c r="H6" t="n">
+        <v>-258</v>
+      </c>
       <c r="I6" t="n">
         <v>-2</v>
       </c>
+      <c r="J6" t="n">
+        <v>102</v>
+      </c>
+      <c r="K6" t="n">
+        <v>2819</v>
+      </c>
       <c r="L6" t="n">
         <v>15031</v>
       </c>
+      <c r="M6" t="n">
+        <v>-78607</v>
+      </c>
       <c r="N6" t="n">
         <v>-0.06</v>
       </c>
@@ -1349,27 +1355,9 @@
           <t>中性</t>
         </is>
       </c>
-      <c r="P6" t="n">
-        <v>6</v>
-      </c>
-      <c r="Q6" s="7" t="n">
-        <v>0.46</v>
-      </c>
-      <c r="R6" t="n">
-        <v>4624000</v>
-      </c>
-      <c r="S6" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="T6" t="n">
-        <v>903.02</v>
-      </c>
-      <c r="U6" t="n">
-        <v>12.95</v>
-      </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>partial</t>
+          <t>N/A</t>
         </is>
       </c>
     </row>
@@ -1387,21 +1375,36 @@
       <c r="C7" t="n">
         <v>40.2</v>
       </c>
-      <c r="D7" s="6" t="n">
+      <c r="D7" s="7" t="n">
         <v>3.47</v>
       </c>
       <c r="E7" t="n">
         <v>96824</v>
       </c>
+      <c r="F7" s="6" t="n">
+        <v>3350</v>
+      </c>
       <c r="G7" t="n">
         <v>-23160</v>
       </c>
+      <c r="H7" t="n">
+        <v>2110</v>
+      </c>
       <c r="I7" t="n">
         <v>-25103</v>
       </c>
+      <c r="J7" t="n">
+        <v>1043</v>
+      </c>
+      <c r="K7" t="n">
+        <v>81314</v>
+      </c>
       <c r="L7" t="n">
         <v>375557</v>
       </c>
+      <c r="M7" t="n">
+        <v>-1104950</v>
+      </c>
       <c r="N7" t="n">
         <v>-0.5</v>
       </c>
@@ -1410,27 +1413,9 @@
           <t>主力積極賣出</t>
         </is>
       </c>
-      <c r="P7" t="n">
-        <v>-31</v>
-      </c>
-      <c r="Q7" s="7" t="n">
-        <v>6.58</v>
-      </c>
-      <c r="R7" t="n">
-        <v>173907918</v>
-      </c>
-      <c r="S7" t="n">
-        <v>1.33</v>
-      </c>
-      <c r="T7" t="n">
-        <v>39.21</v>
-      </c>
-      <c r="U7" t="n">
-        <v>2.52</v>
-      </c>
       <c r="V7" t="inlineStr">
         <is>
-          <t>partial</t>
+          <t>N/A</t>
         </is>
       </c>
     </row>
@@ -1448,21 +1433,36 @@
       <c r="C8" t="n">
         <v>1230</v>
       </c>
-      <c r="D8" s="7" t="n">
+      <c r="D8" s="6" t="n">
         <v>-2.38</v>
       </c>
       <c r="E8" t="n">
         <v>13054</v>
       </c>
+      <c r="F8" s="7" t="n">
+        <v>-2542</v>
+      </c>
       <c r="G8" t="n">
         <v>3149</v>
       </c>
+      <c r="H8" t="n">
+        <v>208</v>
+      </c>
       <c r="I8" t="n">
         <v>802</v>
       </c>
+      <c r="J8" t="n">
+        <v>926</v>
+      </c>
+      <c r="K8" t="n">
+        <v>8406</v>
+      </c>
       <c r="L8" t="n">
         <v>43181</v>
       </c>
+      <c r="M8" t="n">
+        <v>-648525</v>
+      </c>
       <c r="N8" t="n">
         <v>4.41</v>
       </c>
@@ -1471,27 +1471,9 @@
           <t>偏多</t>
         </is>
       </c>
-      <c r="P8" t="n">
-        <v>-41</v>
-      </c>
-      <c r="Q8" s="6" t="n">
-        <v>-0.77</v>
-      </c>
-      <c r="R8" t="n">
-        <v>2009680</v>
-      </c>
-      <c r="S8" t="n">
-        <v>0.13</v>
-      </c>
-      <c r="T8" t="n">
-        <v>1088.59</v>
-      </c>
-      <c r="U8" t="n">
-        <v>12.99</v>
-      </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>partial</t>
+          <t>N/A</t>
         </is>
       </c>
     </row>
@@ -1509,21 +1491,36 @@
       <c r="C9" t="n">
         <v>1755</v>
       </c>
-      <c r="D9" s="7" t="n">
+      <c r="D9" s="6" t="n">
         <v>-0.85</v>
       </c>
       <c r="E9" t="n">
         <v>25989</v>
       </c>
+      <c r="F9" s="7" t="n">
+        <v>-4006</v>
+      </c>
       <c r="G9" t="n">
-        <v>-36793</v>
+        <v>-41711</v>
+      </c>
+      <c r="H9" t="n">
+        <v>-399</v>
       </c>
       <c r="I9" t="n">
-        <v>-4298</v>
+        <v>-934</v>
+      </c>
+      <c r="J9" t="n">
+        <v>705</v>
+      </c>
+      <c r="K9" t="n">
+        <v>20484</v>
       </c>
       <c r="L9" t="n">
         <v>104920</v>
       </c>
+      <c r="M9" t="n">
+        <v>-6482811</v>
+      </c>
       <c r="N9" t="n">
         <v>-0.34</v>
       </c>
@@ -1532,27 +1529,9 @@
           <t>主力積極賣出</t>
         </is>
       </c>
-      <c r="P9" t="n">
-        <v>-17</v>
-      </c>
-      <c r="Q9" s="7" t="n">
-        <v>8.880000000000001</v>
-      </c>
-      <c r="R9" t="n">
-        <v>1586680</v>
-      </c>
-      <c r="S9" t="n">
-        <v>0.04</v>
-      </c>
-      <c r="T9" t="n">
-        <v>1686.05</v>
-      </c>
-      <c r="U9" t="n">
-        <v>4.09</v>
-      </c>
       <c r="V9" t="inlineStr">
         <is>
-          <t>partial</t>
+          <t>N/A</t>
         </is>
       </c>
     </row>
@@ -1570,21 +1549,36 @@
       <c r="C10" t="n">
         <v>113</v>
       </c>
-      <c r="D10" s="6" t="n">
+      <c r="D10" s="7" t="n">
         <v>9.710000000000001</v>
       </c>
       <c r="E10" t="n">
         <v>59539</v>
       </c>
+      <c r="F10" s="7" t="n">
+        <v>-156</v>
+      </c>
       <c r="G10" t="n">
         <v>-18360</v>
       </c>
+      <c r="H10" t="n">
+        <v>-204</v>
+      </c>
       <c r="I10" t="n">
         <v>829</v>
       </c>
+      <c r="J10" t="n">
+        <v>867</v>
+      </c>
+      <c r="K10" t="n">
+        <v>139297</v>
+      </c>
       <c r="L10" t="n">
         <v>675931</v>
       </c>
+      <c r="M10" t="n">
+        <v>-1105127</v>
+      </c>
       <c r="N10" t="n">
         <v>4.15</v>
       </c>
@@ -1593,27 +1587,9 @@
           <t>偏空</t>
         </is>
       </c>
-      <c r="P10" t="n">
-        <v>-30</v>
-      </c>
-      <c r="Q10" s="7" t="n">
-        <v>7.34</v>
-      </c>
-      <c r="R10" t="n">
-        <v>24947000</v>
-      </c>
-      <c r="S10" t="n">
-        <v>0.45</v>
-      </c>
-      <c r="T10" t="n">
-        <v>95.13</v>
-      </c>
-      <c r="U10" t="n">
-        <v>18.78</v>
-      </c>
       <c r="V10" t="inlineStr">
         <is>
-          <t>partial</t>
+          <t>N/A</t>
         </is>
       </c>
     </row>
@@ -1631,21 +1607,36 @@
       <c r="C11" t="n">
         <v>1740</v>
       </c>
-      <c r="D11" s="7" t="n">
+      <c r="D11" s="6" t="n">
         <v>-3.33</v>
       </c>
       <c r="E11" t="n">
         <v>3270</v>
       </c>
+      <c r="F11" s="6" t="n">
+        <v>413</v>
+      </c>
       <c r="G11" t="n">
         <v>5177</v>
       </c>
+      <c r="H11" t="n">
+        <v>-232</v>
+      </c>
       <c r="I11" t="n">
         <v>-1151</v>
       </c>
+      <c r="J11" t="n">
+        <v>161</v>
+      </c>
+      <c r="K11" t="n">
+        <v>2113</v>
+      </c>
       <c r="L11" t="n">
         <v>11575</v>
       </c>
+      <c r="M11" t="n">
+        <v>-89491</v>
+      </c>
       <c r="N11" t="n">
         <v>5.9</v>
       </c>
@@ -1654,27 +1645,9 @@
           <t>中性</t>
         </is>
       </c>
-      <c r="P11" t="n">
-        <v>17</v>
-      </c>
-      <c r="Q11" s="7" t="n">
-        <v>8.91</v>
-      </c>
-      <c r="R11" t="n">
-        <v>2097528</v>
-      </c>
-      <c r="S11" t="n">
-        <v>0.52</v>
-      </c>
-      <c r="T11" t="n">
-        <v>1631.23</v>
-      </c>
-      <c r="U11" t="n">
-        <v>6.67</v>
-      </c>
       <c r="V11" t="inlineStr">
         <is>
-          <t>partial</t>
+          <t>N/A</t>
         </is>
       </c>
     </row>
@@ -1692,21 +1665,36 @@
       <c r="C12" t="n">
         <v>3520</v>
       </c>
-      <c r="D12" s="6" t="n">
+      <c r="D12" s="7" t="n">
         <v>2.62</v>
       </c>
       <c r="E12" t="n">
         <v>1817</v>
       </c>
+      <c r="F12" s="6" t="n">
+        <v>34</v>
+      </c>
       <c r="G12" t="n">
         <v>212</v>
       </c>
+      <c r="H12" t="n">
+        <v>1</v>
+      </c>
       <c r="I12" t="n">
         <v>-208</v>
       </c>
+      <c r="J12" t="n">
+        <v>28</v>
+      </c>
+      <c r="K12" t="n">
+        <v>5744</v>
+      </c>
       <c r="L12" t="n">
         <v>28526</v>
       </c>
+      <c r="M12" t="n">
+        <v>-19711</v>
+      </c>
       <c r="N12" t="n">
         <v>4.92</v>
       </c>
@@ -1715,27 +1703,9 @@
           <t>中性</t>
         </is>
       </c>
-      <c r="P12" t="n">
-        <v>30</v>
-      </c>
-      <c r="Q12" s="6" t="n">
-        <v>-0.8</v>
-      </c>
-      <c r="R12" t="n">
-        <v>4597411</v>
-      </c>
-      <c r="S12" t="n">
-        <v>2.05</v>
-      </c>
-      <c r="T12" t="n">
-        <v>3507.75</v>
-      </c>
-      <c r="U12" t="n">
-        <v>0.35</v>
-      </c>
       <c r="V12" t="inlineStr">
         <is>
-          <t>partial</t>
+          <t>N/A</t>
         </is>
       </c>
     </row>
@@ -1753,21 +1723,36 @@
       <c r="C13" t="n">
         <v>164.5</v>
       </c>
-      <c r="D13" s="7" t="n">
+      <c r="D13" s="6" t="n">
         <v>-3.52</v>
       </c>
       <c r="E13" t="n">
         <v>8266</v>
       </c>
+      <c r="F13" s="7" t="n">
+        <v>-3616</v>
+      </c>
       <c r="G13" t="n">
         <v>-2738</v>
       </c>
+      <c r="H13" t="n">
+        <v>-119</v>
+      </c>
       <c r="I13" t="n">
         <v>312</v>
       </c>
+      <c r="J13" t="n">
+        <v>261</v>
+      </c>
+      <c r="K13" t="n">
+        <v>19888</v>
+      </c>
       <c r="L13" t="n">
         <v>109999</v>
       </c>
+      <c r="M13" t="n">
+        <v>-267533</v>
+      </c>
       <c r="N13" t="n">
         <v>-0.84</v>
       </c>
@@ -1776,27 +1761,9 @@
           <t>偏空</t>
         </is>
       </c>
-      <c r="P13" t="n">
-        <v>-21</v>
-      </c>
-      <c r="Q13" s="6" t="n">
-        <v>-0.36</v>
-      </c>
-      <c r="R13" t="n">
-        <v>16043945</v>
-      </c>
-      <c r="S13" t="n">
-        <v>0.78</v>
-      </c>
-      <c r="T13" t="n">
-        <v>163.51</v>
-      </c>
-      <c r="U13" t="n">
-        <v>0.61</v>
-      </c>
       <c r="V13" t="inlineStr">
         <is>
-          <t>partial</t>
+          <t>N/A</t>
         </is>
       </c>
     </row>
@@ -1814,21 +1781,36 @@
       <c r="C14" t="n">
         <v>1300</v>
       </c>
-      <c r="D14" s="7" t="n">
+      <c r="D14" s="6" t="n">
         <v>-4.06</v>
       </c>
       <c r="E14" t="n">
         <v>3290</v>
       </c>
+      <c r="F14" s="7" t="n">
+        <v>-751</v>
+      </c>
       <c r="G14" t="n">
         <v>680</v>
       </c>
+      <c r="H14" t="n">
+        <v>25</v>
+      </c>
       <c r="I14" t="n">
         <v>302</v>
       </c>
+      <c r="J14" t="n">
+        <v>66</v>
+      </c>
+      <c r="K14" t="n">
+        <v>5059</v>
+      </c>
       <c r="L14" t="n">
         <v>25765</v>
       </c>
+      <c r="M14" t="n">
+        <v>-19195</v>
+      </c>
       <c r="N14" t="n">
         <v>1.48</v>
       </c>
@@ -1837,27 +1819,9 @@
           <t>偏多</t>
         </is>
       </c>
-      <c r="P14" t="n">
-        <v>44</v>
-      </c>
-      <c r="Q14" s="7" t="n">
-        <v>2.22</v>
-      </c>
-      <c r="R14" t="n">
-        <v>2162000</v>
-      </c>
-      <c r="S14" t="n">
-        <v>0.61</v>
-      </c>
-      <c r="T14" t="n">
-        <v>1335.28</v>
-      </c>
-      <c r="U14" t="n">
-        <v>-2.64</v>
-      </c>
       <c r="V14" t="inlineStr">
         <is>
-          <t>partial</t>
+          <t>N/A</t>
         </is>
       </c>
     </row>
@@ -1875,21 +1839,36 @@
       <c r="C15" t="n">
         <v>1000</v>
       </c>
-      <c r="D15" s="7" t="n">
+      <c r="D15" s="6" t="n">
         <v>-2.44</v>
       </c>
       <c r="E15" t="n">
         <v>905</v>
       </c>
+      <c r="F15" s="7" t="n">
+        <v>-260</v>
+      </c>
       <c r="G15" t="n">
         <v>1656</v>
       </c>
+      <c r="H15" t="n">
+        <v>78</v>
+      </c>
       <c r="I15" t="n">
         <v>1022</v>
       </c>
+      <c r="J15" t="n">
+        <v>19</v>
+      </c>
+      <c r="K15" t="n">
+        <v>46</v>
+      </c>
       <c r="L15" t="n">
         <v>-753</v>
       </c>
+      <c r="M15" t="n">
+        <v>0</v>
+      </c>
       <c r="N15" t="n">
         <v>0</v>
       </c>
@@ -1898,27 +1877,9 @@
           <t>主力積極買進</t>
         </is>
       </c>
-      <c r="P15" t="n">
-        <v>-15</v>
-      </c>
-      <c r="Q15" s="6" t="n">
-        <v>-1.68</v>
-      </c>
-      <c r="R15" t="n">
-        <v>2733400</v>
-      </c>
-      <c r="S15" t="n">
-        <v>3.02</v>
-      </c>
-      <c r="T15" t="n">
-        <v>711.84</v>
-      </c>
-      <c r="U15" t="n">
-        <v>40.48</v>
-      </c>
       <c r="V15" t="inlineStr">
         <is>
-          <t>partial</t>
+          <t>N/A</t>
         </is>
       </c>
     </row>
@@ -1936,21 +1897,36 @@
       <c r="C16" t="n">
         <v>306.5</v>
       </c>
-      <c r="D16" s="7" t="n">
+      <c r="D16" s="6" t="n">
         <v>-8.1</v>
       </c>
       <c r="E16" t="n">
         <v>26486</v>
       </c>
+      <c r="F16" s="7" t="n">
+        <v>-1622</v>
+      </c>
       <c r="G16" t="n">
         <v>-373</v>
       </c>
+      <c r="H16" t="n">
+        <v>-42</v>
+      </c>
       <c r="I16" t="n">
         <v>-668</v>
       </c>
+      <c r="J16" t="n">
+        <v>-63</v>
+      </c>
+      <c r="K16" t="n">
+        <v>2325</v>
+      </c>
       <c r="L16" t="n">
         <v>3391</v>
       </c>
+      <c r="M16" t="n">
+        <v>0</v>
+      </c>
       <c r="N16" t="n">
         <v>0</v>
       </c>
@@ -1959,27 +1935,9 @@
           <t>主力積極賣出</t>
         </is>
       </c>
-      <c r="P16" t="n">
-        <v>40</v>
-      </c>
-      <c r="Q16" s="6" t="n">
-        <v>-3.53</v>
-      </c>
-      <c r="R16" t="n">
-        <v>6292640</v>
-      </c>
-      <c r="S16" t="n">
-        <v>0.24</v>
-      </c>
-      <c r="T16" t="n">
-        <v>276.93</v>
-      </c>
-      <c r="U16" t="n">
-        <v>10.68</v>
-      </c>
       <c r="V16" t="inlineStr">
         <is>
-          <t>partial</t>
+          <t>N/A</t>
         </is>
       </c>
     </row>
@@ -1997,21 +1955,36 @@
       <c r="C17" t="n">
         <v>132.5</v>
       </c>
-      <c r="D17" s="7" t="n">
+      <c r="D17" s="6" t="n">
         <v>-2.57</v>
       </c>
       <c r="E17" t="n">
         <v>1591</v>
       </c>
+      <c r="F17" s="6" t="n">
+        <v>507</v>
+      </c>
       <c r="G17" t="n">
         <v>996</v>
       </c>
+      <c r="H17" t="n">
+        <v>346</v>
+      </c>
       <c r="I17" t="n">
         <v>462</v>
       </c>
+      <c r="J17" t="n">
+        <v>199</v>
+      </c>
+      <c r="K17" t="n">
+        <v>74</v>
+      </c>
       <c r="L17" t="n">
         <v>-956</v>
       </c>
+      <c r="M17" t="n">
+        <v>0</v>
+      </c>
       <c r="N17" t="n">
         <v>0</v>
       </c>
@@ -2020,27 +1993,9 @@
           <t>主力積極買進</t>
         </is>
       </c>
-      <c r="P17" t="n">
-        <v>-13</v>
-      </c>
-      <c r="Q17" s="6" t="n">
-        <v>-7.64</v>
-      </c>
-      <c r="R17" t="n">
-        <v>2432000</v>
-      </c>
-      <c r="S17" t="n">
-        <v>1.53</v>
-      </c>
-      <c r="T17" t="n">
-        <v>134.7</v>
-      </c>
-      <c r="U17" t="n">
-        <v>-1.63</v>
-      </c>
       <c r="V17" t="inlineStr">
         <is>
-          <t>partial</t>
+          <t>N/A</t>
         </is>
       </c>
     </row>
@@ -2058,21 +2013,36 @@
       <c r="C18" t="n">
         <v>318.5</v>
       </c>
-      <c r="D18" s="7" t="n">
+      <c r="D18" s="6" t="n">
         <v>-0.16</v>
       </c>
       <c r="E18" t="n">
         <v>20497</v>
       </c>
+      <c r="F18" s="7" t="n">
+        <v>-1587</v>
+      </c>
       <c r="G18" t="n">
         <v>-5684</v>
       </c>
+      <c r="H18" t="n">
+        <v>72</v>
+      </c>
       <c r="I18" t="n">
         <v>3009</v>
       </c>
+      <c r="J18" t="n">
+        <v>-31</v>
+      </c>
+      <c r="K18" t="n">
+        <v>-696</v>
+      </c>
       <c r="L18" t="n">
         <v>-78</v>
       </c>
+      <c r="M18" t="n">
+        <v>0</v>
+      </c>
       <c r="N18" t="n">
         <v>0</v>
       </c>
@@ -2081,27 +2051,9 @@
           <t>中性</t>
         </is>
       </c>
-      <c r="P18" t="n">
-        <v>33</v>
-      </c>
-      <c r="Q18" s="6" t="n">
-        <v>-2.63</v>
-      </c>
-      <c r="R18" t="n">
-        <v>11889993</v>
-      </c>
-      <c r="S18" t="n">
-        <v>0.58</v>
-      </c>
-      <c r="T18" t="n">
-        <v>298.63</v>
-      </c>
-      <c r="U18" t="n">
-        <v>6.65</v>
-      </c>
       <c r="V18" t="inlineStr">
         <is>
-          <t>partial</t>
+          <t>N/A</t>
         </is>
       </c>
     </row>
@@ -2125,15 +2077,30 @@
       <c r="E19" t="n">
         <v>21470</v>
       </c>
+      <c r="F19" s="7" t="n">
+        <v>-1260</v>
+      </c>
       <c r="G19" t="n">
         <v>-16551</v>
       </c>
+      <c r="H19" t="n">
+        <v>384</v>
+      </c>
       <c r="I19" t="n">
         <v>8081</v>
       </c>
+      <c r="J19" t="n">
+        <v>1538</v>
+      </c>
+      <c r="K19" t="n">
+        <v>32493</v>
+      </c>
       <c r="L19" t="n">
         <v>153230</v>
       </c>
+      <c r="M19" t="n">
+        <v>-114150</v>
+      </c>
       <c r="N19" t="n">
         <v>0.24</v>
       </c>
@@ -2142,27 +2109,9 @@
           <t>偏空</t>
         </is>
       </c>
-      <c r="P19" t="n">
-        <v>-6</v>
-      </c>
-      <c r="Q19" s="6" t="n">
-        <v>-1.6</v>
-      </c>
-      <c r="R19" t="n">
-        <v>5270826</v>
-      </c>
-      <c r="S19" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="T19" t="n">
-        <v>186.56</v>
-      </c>
-      <c r="U19" t="n">
-        <v>11.49</v>
-      </c>
       <c r="V19" t="inlineStr">
         <is>
-          <t>partial</t>
+          <t>N/A</t>
         </is>
       </c>
     </row>

</xml_diff>